<commit_message>
readding full data folder after reclone
</commit_message>
<xml_diff>
--- a/data/00_metadata/age data/Fall2023_haddock_finclips_aged.xlsx
+++ b/data/00_metadata/age data/Fall2023_haddock_finclips_aged.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eric.robillard\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BoxDrive\Box\Science\Fisheries\Projects\Epigenetic Aging\github\Epigenetic_aging_haddock\data\00_metadata\age data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8834B007-9947-4CEB-9804-03E8FF667924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fall 2023 haddock" sheetId="1" r:id="rId1"/>
@@ -1920,7 +1921,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2723,14 +2724,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S400"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2789,7 +2792,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>202304</v>
       </c>
@@ -2842,7 +2845,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>202304</v>
       </c>
@@ -2895,7 +2898,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>202304</v>
       </c>
@@ -2942,7 +2945,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>202304</v>
       </c>
@@ -2995,7 +2998,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>202304</v>
       </c>
@@ -3048,7 +3051,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>202304</v>
       </c>
@@ -3101,7 +3104,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>202304</v>
       </c>
@@ -3154,7 +3157,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>202304</v>
       </c>
@@ -3207,7 +3210,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>202304</v>
       </c>
@@ -3260,7 +3263,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>202304</v>
       </c>
@@ -3310,7 +3313,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>202304</v>
       </c>
@@ -3363,7 +3366,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>202304</v>
       </c>
@@ -3413,7 +3416,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>202304</v>
       </c>
@@ -3463,7 +3466,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>202304</v>
       </c>
@@ -3516,7 +3519,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>202304</v>
       </c>
@@ -3566,7 +3569,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>202304</v>
       </c>
@@ -3616,7 +3619,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>202304</v>
       </c>
@@ -3669,7 +3672,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>202304</v>
       </c>
@@ -3719,7 +3722,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>202304</v>
       </c>
@@ -3769,7 +3772,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>202304</v>
       </c>
@@ -3819,7 +3822,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>202304</v>
       </c>
@@ -3869,7 +3872,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>202304</v>
       </c>
@@ -3919,7 +3922,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>202304</v>
       </c>
@@ -3969,7 +3972,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>202304</v>
       </c>
@@ -4022,7 +4025,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>202304</v>
       </c>
@@ -4072,7 +4075,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>202304</v>
       </c>
@@ -4122,7 +4125,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>202304</v>
       </c>
@@ -4172,7 +4175,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>202304</v>
       </c>
@@ -4222,7 +4225,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>202304</v>
       </c>
@@ -4272,7 +4275,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>202304</v>
       </c>
@@ -4322,7 +4325,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>202304</v>
       </c>
@@ -4372,7 +4375,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>202304</v>
       </c>
@@ -4422,7 +4425,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>202304</v>
       </c>
@@ -4472,7 +4475,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>202304</v>
       </c>
@@ -4522,7 +4525,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>202304</v>
       </c>
@@ -4572,7 +4575,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>202304</v>
       </c>
@@ -4622,7 +4625,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>202304</v>
       </c>
@@ -4672,7 +4675,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>202304</v>
       </c>
@@ -4722,7 +4725,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>202304</v>
       </c>
@@ -4772,7 +4775,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>202304</v>
       </c>
@@ -4822,7 +4825,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>202304</v>
       </c>
@@ -4872,7 +4875,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>202304</v>
       </c>
@@ -4922,7 +4925,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>202304</v>
       </c>
@@ -4975,7 +4978,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>202304</v>
       </c>
@@ -5025,7 +5028,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>202304</v>
       </c>
@@ -5075,7 +5078,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>202304</v>
       </c>
@@ -5125,7 +5128,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>202304</v>
       </c>
@@ -5175,7 +5178,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>202304</v>
       </c>
@@ -5231,7 +5234,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>202304</v>
       </c>
@@ -5281,7 +5284,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>202304</v>
       </c>
@@ -5331,7 +5334,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>202304</v>
       </c>
@@ -5381,7 +5384,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>202304</v>
       </c>
@@ -5431,7 +5434,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>202304</v>
       </c>
@@ -5481,7 +5484,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>202304</v>
       </c>
@@ -5537,7 +5540,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>202304</v>
       </c>
@@ -5587,7 +5590,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>202304</v>
       </c>
@@ -5637,7 +5640,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>202304</v>
       </c>
@@ -5687,7 +5690,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>202304</v>
       </c>
@@ -5737,7 +5740,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>202304</v>
       </c>
@@ -5787,7 +5790,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>202304</v>
       </c>
@@ -5837,7 +5840,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>202304</v>
       </c>
@@ -5887,7 +5890,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>202304</v>
       </c>
@@ -5940,7 +5943,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>202304</v>
       </c>
@@ -5990,7 +5993,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>202304</v>
       </c>
@@ -6040,7 +6043,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>202304</v>
       </c>
@@ -6090,7 +6093,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>202304</v>
       </c>
@@ -6143,7 +6146,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>202304</v>
       </c>
@@ -6193,7 +6196,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>202304</v>
       </c>
@@ -6243,7 +6246,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>202304</v>
       </c>
@@ -6293,7 +6296,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>202304</v>
       </c>
@@ -6340,7 +6343,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>202304</v>
       </c>
@@ -6390,7 +6393,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>202304</v>
       </c>
@@ -6440,7 +6443,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>202304</v>
       </c>
@@ -6490,7 +6493,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>202304</v>
       </c>
@@ -6537,7 +6540,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>202304</v>
       </c>
@@ -6587,7 +6590,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>202304</v>
       </c>
@@ -6637,7 +6640,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>202304</v>
       </c>
@@ -6687,7 +6690,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>202304</v>
       </c>
@@ -6737,7 +6740,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>202304</v>
       </c>
@@ -6787,7 +6790,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>202304</v>
       </c>
@@ -6840,7 +6843,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>202304</v>
       </c>
@@ -6890,7 +6893,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>202304</v>
       </c>
@@ -6940,7 +6943,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>202304</v>
       </c>
@@ -6987,7 +6990,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>202304</v>
       </c>
@@ -7037,7 +7040,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>202304</v>
       </c>
@@ -7087,7 +7090,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>202304</v>
       </c>
@@ -7137,7 +7140,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>202304</v>
       </c>
@@ -7187,7 +7190,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>202304</v>
       </c>
@@ -7237,7 +7240,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>202304</v>
       </c>
@@ -7287,7 +7290,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>202304</v>
       </c>
@@ -7340,7 +7343,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>202304</v>
       </c>
@@ -7390,7 +7393,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>202304</v>
       </c>
@@ -7440,7 +7443,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>202304</v>
       </c>
@@ -7490,7 +7493,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>202304</v>
       </c>
@@ -7540,7 +7543,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>202304</v>
       </c>
@@ -7590,7 +7593,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>202304</v>
       </c>
@@ -7640,7 +7643,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>202304</v>
       </c>
@@ -7690,7 +7693,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>202304</v>
       </c>
@@ -7737,7 +7740,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>202304</v>
       </c>
@@ -7784,7 +7787,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>202304</v>
       </c>
@@ -7831,7 +7834,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>202304</v>
       </c>
@@ -7878,7 +7881,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>202304</v>
       </c>
@@ -7925,7 +7928,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>202304</v>
       </c>
@@ -7972,7 +7975,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>202304</v>
       </c>
@@ -8025,7 +8028,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>202304</v>
       </c>
@@ -8072,7 +8075,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>202304</v>
       </c>
@@ -8119,7 +8122,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>202304</v>
       </c>
@@ -8166,7 +8169,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>202304</v>
       </c>
@@ -8213,7 +8216,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>202304</v>
       </c>
@@ -8263,7 +8266,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>202304</v>
       </c>
@@ -8313,7 +8316,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>202304</v>
       </c>
@@ -8366,7 +8369,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>202304</v>
       </c>
@@ -8419,7 +8422,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>202304</v>
       </c>
@@ -8469,7 +8472,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>202304</v>
       </c>
@@ -8522,7 +8525,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>202304</v>
       </c>
@@ -8572,7 +8575,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>202304</v>
       </c>
@@ -8622,7 +8625,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>202304</v>
       </c>
@@ -8672,7 +8675,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>202304</v>
       </c>
@@ -8722,7 +8725,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>202304</v>
       </c>
@@ -8772,7 +8775,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>202304</v>
       </c>
@@ -8822,7 +8825,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>202304</v>
       </c>
@@ -8872,7 +8875,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>202304</v>
       </c>
@@ -8922,7 +8925,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>202304</v>
       </c>
@@ -8978,7 +8981,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>202304</v>
       </c>
@@ -9028,7 +9031,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>202304</v>
       </c>
@@ -9078,7 +9081,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>202304</v>
       </c>
@@ -9128,7 +9131,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>202304</v>
       </c>
@@ -9178,7 +9181,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>202304</v>
       </c>
@@ -9228,7 +9231,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>202304</v>
       </c>
@@ -9278,7 +9281,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>202304</v>
       </c>
@@ -9334,7 +9337,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>202304</v>
       </c>
@@ -9384,7 +9387,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>202304</v>
       </c>
@@ -9434,7 +9437,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>202304</v>
       </c>
@@ -9484,7 +9487,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>202304</v>
       </c>
@@ -9537,7 +9540,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>202304</v>
       </c>
@@ -9587,7 +9590,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>202304</v>
       </c>
@@ -9637,7 +9640,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>202304</v>
       </c>
@@ -9687,7 +9690,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>202304</v>
       </c>
@@ -9734,7 +9737,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="140" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>202304</v>
       </c>
@@ -9784,7 +9787,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="141" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>202304</v>
       </c>
@@ -9834,7 +9837,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="142" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>202304</v>
       </c>
@@ -9884,7 +9887,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="143" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>202304</v>
       </c>
@@ -9937,7 +9940,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="144" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>202304</v>
       </c>
@@ -9993,7 +9996,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="145" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>202304</v>
       </c>
@@ -10046,7 +10049,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="146" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>202304</v>
       </c>
@@ -10096,7 +10099,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="147" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>202304</v>
       </c>
@@ -10146,7 +10149,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="148" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>202304</v>
       </c>
@@ -10196,7 +10199,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="149" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>202304</v>
       </c>
@@ -10246,7 +10249,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="150" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>202304</v>
       </c>
@@ -10296,7 +10299,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="151" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>202304</v>
       </c>
@@ -10346,7 +10349,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="152" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>202304</v>
       </c>
@@ -10396,7 +10399,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="153" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>202304</v>
       </c>
@@ -10446,7 +10449,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="154" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>202304</v>
       </c>
@@ -10496,7 +10499,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="155" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>202304</v>
       </c>
@@ -10546,7 +10549,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="156" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>202304</v>
       </c>
@@ -10596,7 +10599,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="157" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>202304</v>
       </c>
@@ -10646,7 +10649,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="158" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>202304</v>
       </c>
@@ -10699,7 +10702,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="159" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>202304</v>
       </c>
@@ -10749,7 +10752,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="160" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>202304</v>
       </c>
@@ -10799,7 +10802,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="161" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>202304</v>
       </c>
@@ -10849,7 +10852,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="162" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>202304</v>
       </c>
@@ -10899,7 +10902,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="163" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>202304</v>
       </c>
@@ -10949,7 +10952,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="164" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>202304</v>
       </c>
@@ -10999,7 +11002,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="165" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>202304</v>
       </c>
@@ -11049,7 +11052,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="166" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>202304</v>
       </c>
@@ -11105,7 +11108,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="167" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>202304</v>
       </c>
@@ -11155,7 +11158,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="168" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>202304</v>
       </c>
@@ -11205,7 +11208,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="169" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>202304</v>
       </c>
@@ -11261,7 +11264,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="170" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>202304</v>
       </c>
@@ -11311,7 +11314,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="171" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>202304</v>
       </c>
@@ -11361,7 +11364,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="172" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>202304</v>
       </c>
@@ -11411,7 +11414,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="173" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>202304</v>
       </c>
@@ -11461,7 +11464,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="174" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>202304</v>
       </c>
@@ -11514,7 +11517,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="175" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>202304</v>
       </c>
@@ -11564,7 +11567,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="176" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>202304</v>
       </c>
@@ -11614,7 +11617,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="177" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>202304</v>
       </c>
@@ -11670,7 +11673,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="178" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>202304</v>
       </c>
@@ -11723,7 +11726,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="179" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>202304</v>
       </c>
@@ -11776,7 +11779,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="180" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>202304</v>
       </c>
@@ -11832,7 +11835,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="181" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>202304</v>
       </c>
@@ -11882,7 +11885,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="182" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>202304</v>
       </c>
@@ -11932,7 +11935,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="183" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>202304</v>
       </c>
@@ -11979,7 +11982,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="184" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>202304</v>
       </c>
@@ -12029,7 +12032,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="185" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>202304</v>
       </c>
@@ -12079,7 +12082,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="186" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>202304</v>
       </c>
@@ -12129,7 +12132,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="187" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>202304</v>
       </c>
@@ -12179,7 +12182,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="188" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>202304</v>
       </c>
@@ -12229,7 +12232,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="189" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>202304</v>
       </c>
@@ -12279,7 +12282,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="190" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>202304</v>
       </c>
@@ -12335,7 +12338,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="191" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>202304</v>
       </c>
@@ -12388,7 +12391,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="192" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>202304</v>
       </c>
@@ -12438,7 +12441,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="193" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>202304</v>
       </c>
@@ -12488,7 +12491,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="194" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>202304</v>
       </c>
@@ -12538,7 +12541,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="195" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>202304</v>
       </c>
@@ -12588,7 +12591,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="196" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>202304</v>
       </c>
@@ -12638,7 +12641,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="197" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>202304</v>
       </c>
@@ -12688,7 +12691,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="198" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>202304</v>
       </c>
@@ -12738,7 +12741,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="199" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>202304</v>
       </c>
@@ -12788,7 +12791,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="200" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>202304</v>
       </c>
@@ -12838,7 +12841,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="201" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>202304</v>
       </c>
@@ -12891,7 +12894,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="202" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>202304</v>
       </c>
@@ -12947,7 +12950,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="203" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>202304</v>
       </c>
@@ -12997,7 +13000,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="204" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>202304</v>
       </c>
@@ -13047,7 +13050,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="205" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>202304</v>
       </c>
@@ -13097,7 +13100,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="206" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>202304</v>
       </c>
@@ -13147,7 +13150,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="207" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>202304</v>
       </c>
@@ -13200,7 +13203,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="208" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>202304</v>
       </c>
@@ -13256,7 +13259,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="209" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>202304</v>
       </c>
@@ -13306,7 +13309,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="210" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>202304</v>
       </c>
@@ -13362,7 +13365,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="211" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>202304</v>
       </c>
@@ -13412,7 +13415,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="212" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>202304</v>
       </c>
@@ -13462,7 +13465,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="213" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>202304</v>
       </c>
@@ -13512,7 +13515,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="214" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>202304</v>
       </c>
@@ -13565,7 +13568,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="215" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>202304</v>
       </c>
@@ -13615,7 +13618,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="216" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>202304</v>
       </c>
@@ -13665,7 +13668,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="217" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>202304</v>
       </c>
@@ -13721,7 +13724,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="218" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>202304</v>
       </c>
@@ -13771,7 +13774,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="219" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>202304</v>
       </c>
@@ -13821,7 +13824,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="220" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>202304</v>
       </c>
@@ -13871,7 +13874,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="221" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>202304</v>
       </c>
@@ -13921,7 +13924,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="222" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>202304</v>
       </c>
@@ -13968,7 +13971,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="223" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>202304</v>
       </c>
@@ -14018,7 +14021,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="224" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>202304</v>
       </c>
@@ -14071,7 +14074,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="225" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>202304</v>
       </c>
@@ -14121,7 +14124,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="226" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>202304</v>
       </c>
@@ -14171,7 +14174,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="227" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>202304</v>
       </c>
@@ -14221,7 +14224,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="228" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>202304</v>
       </c>
@@ -14274,7 +14277,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="229" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>202304</v>
       </c>
@@ -14324,7 +14327,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="230" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>202304</v>
       </c>
@@ -14374,7 +14377,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="231" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>202304</v>
       </c>
@@ -14424,7 +14427,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="232" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>202304</v>
       </c>
@@ -14474,7 +14477,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="233" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>202304</v>
       </c>
@@ -14524,7 +14527,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="234" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>202304</v>
       </c>
@@ -14574,7 +14577,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="235" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>202304</v>
       </c>
@@ -14624,7 +14627,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="236" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>202304</v>
       </c>
@@ -14674,7 +14677,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="237" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>202304</v>
       </c>
@@ -14724,7 +14727,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="238" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>202304</v>
       </c>
@@ -14774,7 +14777,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="239" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>202304</v>
       </c>
@@ -14827,7 +14830,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="240" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>202304</v>
       </c>
@@ -14877,7 +14880,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="241" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>202304</v>
       </c>
@@ -14927,7 +14930,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="242" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>202304</v>
       </c>
@@ -14983,7 +14986,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="243" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>202304</v>
       </c>
@@ -15033,7 +15036,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="244" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>202304</v>
       </c>
@@ -15083,7 +15086,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="245" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>202304</v>
       </c>
@@ -15133,7 +15136,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="246" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>202304</v>
       </c>
@@ -15183,7 +15186,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="247" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>202304</v>
       </c>
@@ -15239,7 +15242,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="248" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>202304</v>
       </c>
@@ -15289,7 +15292,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="249" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>202304</v>
       </c>
@@ -15342,7 +15345,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="250" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>202304</v>
       </c>
@@ -15392,7 +15395,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="251" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>202304</v>
       </c>
@@ -15442,7 +15445,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="252" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>202304</v>
       </c>
@@ -15492,7 +15495,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="253" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>202304</v>
       </c>
@@ -15545,7 +15548,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="254" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>202304</v>
       </c>
@@ -15595,7 +15598,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="255" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>202304</v>
       </c>
@@ -15645,7 +15648,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="256" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>202304</v>
       </c>
@@ -15695,7 +15698,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="257" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>202304</v>
       </c>
@@ -15745,7 +15748,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="258" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>202304</v>
       </c>
@@ -15798,7 +15801,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="259" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>202304</v>
       </c>
@@ -15851,7 +15854,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="260" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>202304</v>
       </c>
@@ -15901,7 +15904,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="261" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>202304</v>
       </c>
@@ -15951,7 +15954,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="262" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>202304</v>
       </c>
@@ -16007,7 +16010,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="263" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>202304</v>
       </c>
@@ -16057,7 +16060,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="264" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>202304</v>
       </c>
@@ -16107,7 +16110,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="265" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>202304</v>
       </c>
@@ -16157,7 +16160,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="266" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>202304</v>
       </c>
@@ -16207,7 +16210,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="267" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>202304</v>
       </c>
@@ -16260,7 +16263,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="268" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>202304</v>
       </c>
@@ -16310,7 +16313,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="269" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>202304</v>
       </c>
@@ -16360,7 +16363,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="270" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>202304</v>
       </c>
@@ -16410,7 +16413,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="271" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>202304</v>
       </c>
@@ -16466,7 +16469,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="272" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>202304</v>
       </c>
@@ -16519,7 +16522,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="273" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>202304</v>
       </c>
@@ -16569,7 +16572,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="274" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>202304</v>
       </c>
@@ -16619,7 +16622,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="275" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>202304</v>
       </c>
@@ -16669,7 +16672,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="276" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>202304</v>
       </c>
@@ -16719,7 +16722,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="277" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>202304</v>
       </c>
@@ -16775,7 +16778,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="278" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>202304</v>
       </c>
@@ -16825,7 +16828,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="279" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>202304</v>
       </c>
@@ -16881,7 +16884,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="280" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>202304</v>
       </c>
@@ -16931,7 +16934,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="281" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>202304</v>
       </c>
@@ -16981,7 +16984,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="282" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>202304</v>
       </c>
@@ -17034,7 +17037,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="283" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>202304</v>
       </c>
@@ -17084,7 +17087,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="284" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>202304</v>
       </c>
@@ -17137,7 +17140,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="285" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>202304</v>
       </c>
@@ -17187,7 +17190,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="286" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>202304</v>
       </c>
@@ -17237,7 +17240,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="287" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>202304</v>
       </c>
@@ -17284,7 +17287,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="288" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A288">
         <v>202304</v>
       </c>
@@ -17334,7 +17337,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="289" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>202304</v>
       </c>
@@ -17384,7 +17387,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="290" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>202304</v>
       </c>
@@ -17434,7 +17437,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="291" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>202304</v>
       </c>
@@ -17487,7 +17490,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="292" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>202304</v>
       </c>
@@ -17543,7 +17546,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="293" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>202304</v>
       </c>
@@ -17593,7 +17596,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="294" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>202304</v>
       </c>
@@ -17649,7 +17652,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="295" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>202304</v>
       </c>
@@ -17699,7 +17702,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="296" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>202304</v>
       </c>
@@ -17749,7 +17752,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="297" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>202304</v>
       </c>
@@ -17805,7 +17808,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="298" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>202304</v>
       </c>
@@ -17861,7 +17864,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="299" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>202304</v>
       </c>
@@ -17911,7 +17914,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="300" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>202304</v>
       </c>
@@ -17967,7 +17970,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="301" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A301">
         <v>202304</v>
       </c>
@@ -18017,7 +18020,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="302" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A302">
         <v>202304</v>
       </c>
@@ -18067,7 +18070,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="303" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A303">
         <v>202304</v>
       </c>
@@ -18120,7 +18123,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="304" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A304">
         <v>202304</v>
       </c>
@@ -18173,7 +18176,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="305" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A305">
         <v>202304</v>
       </c>
@@ -18223,7 +18226,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="306" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A306">
         <v>202304</v>
       </c>
@@ -18273,7 +18276,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="307" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A307">
         <v>202304</v>
       </c>
@@ -18323,7 +18326,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="308" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A308">
         <v>202304</v>
       </c>
@@ -18373,7 +18376,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="309" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A309">
         <v>202304</v>
       </c>
@@ -18423,7 +18426,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="310" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A310">
         <v>202304</v>
       </c>
@@ -18473,7 +18476,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="311" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A311">
         <v>202304</v>
       </c>
@@ -18523,7 +18526,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="312" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A312">
         <v>202304</v>
       </c>
@@ -18576,7 +18579,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="313" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A313">
         <v>202304</v>
       </c>
@@ -18626,7 +18629,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="314" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A314">
         <v>202304</v>
       </c>
@@ -18676,7 +18679,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="315" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A315">
         <v>202304</v>
       </c>
@@ -18726,7 +18729,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="316" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A316">
         <v>202304</v>
       </c>
@@ -18782,7 +18785,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="317" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A317">
         <v>202304</v>
       </c>
@@ -18832,7 +18835,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="318" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A318">
         <v>202304</v>
       </c>
@@ -18882,7 +18885,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="319" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A319">
         <v>202304</v>
       </c>
@@ -18932,7 +18935,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="320" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A320">
         <v>202304</v>
       </c>
@@ -18982,7 +18985,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="321" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A321">
         <v>202304</v>
       </c>
@@ -19035,7 +19038,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="322" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A322">
         <v>202304</v>
       </c>
@@ -19085,7 +19088,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="323" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A323">
         <v>202304</v>
       </c>
@@ -19132,7 +19135,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="324" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A324">
         <v>202304</v>
       </c>
@@ -19182,7 +19185,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="325" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A325">
         <v>202304</v>
       </c>
@@ -19232,7 +19235,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="326" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A326">
         <v>202304</v>
       </c>
@@ -19282,7 +19285,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="327" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A327">
         <v>202304</v>
       </c>
@@ -19335,7 +19338,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="328" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A328">
         <v>202304</v>
       </c>
@@ -19391,7 +19394,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="329" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A329">
         <v>202304</v>
       </c>
@@ -19441,7 +19444,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="330" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A330">
         <v>202304</v>
       </c>
@@ -19491,7 +19494,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="331" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A331">
         <v>202304</v>
       </c>
@@ -19541,7 +19544,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="332" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A332">
         <v>202304</v>
       </c>
@@ -19591,7 +19594,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="333" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A333">
         <v>202304</v>
       </c>
@@ -19641,7 +19644,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="334" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A334">
         <v>202304</v>
       </c>
@@ -19691,7 +19694,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="335" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A335">
         <v>202304</v>
       </c>
@@ -19747,7 +19750,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="336" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A336">
         <v>202304</v>
       </c>
@@ -19800,7 +19803,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="337" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A337">
         <v>202304</v>
       </c>
@@ -19850,7 +19853,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="338" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A338">
         <v>202304</v>
       </c>
@@ -19900,7 +19903,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="339" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A339">
         <v>202304</v>
       </c>
@@ -19950,7 +19953,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="340" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A340">
         <v>202304</v>
       </c>
@@ -20000,7 +20003,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="341" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A341">
         <v>202304</v>
       </c>
@@ -20050,7 +20053,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="342" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A342">
         <v>202304</v>
       </c>
@@ -20100,7 +20103,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="343" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A343">
         <v>202304</v>
       </c>
@@ -20150,7 +20153,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="344" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A344">
         <v>202304</v>
       </c>
@@ -20200,7 +20203,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="345" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A345">
         <v>202304</v>
       </c>
@@ -20250,7 +20253,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="346" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A346">
         <v>202304</v>
       </c>
@@ -20300,7 +20303,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="347" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A347">
         <v>202304</v>
       </c>
@@ -20353,7 +20356,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="348" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A348">
         <v>202304</v>
       </c>
@@ -20403,7 +20406,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="349" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A349">
         <v>202304</v>
       </c>
@@ -20453,7 +20456,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="350" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A350">
         <v>202304</v>
       </c>
@@ -20509,7 +20512,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="351" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A351">
         <v>202304</v>
       </c>
@@ -20559,7 +20562,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="352" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A352">
         <v>202304</v>
       </c>
@@ -20612,7 +20615,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="353" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A353">
         <v>202304</v>
       </c>
@@ -20662,7 +20665,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="354" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A354">
         <v>202304</v>
       </c>
@@ -20715,7 +20718,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="355" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A355">
         <v>202304</v>
       </c>
@@ -20765,7 +20768,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="356" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A356">
         <v>202304</v>
       </c>
@@ -20812,7 +20815,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="357" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A357">
         <v>202304</v>
       </c>
@@ -20868,7 +20871,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="358" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A358">
         <v>202304</v>
       </c>
@@ -20915,7 +20918,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="359" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A359">
         <v>202304</v>
       </c>
@@ -20962,7 +20965,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="360" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A360">
         <v>202304</v>
       </c>
@@ -21012,7 +21015,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="361" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A361">
         <v>202304</v>
       </c>
@@ -21068,7 +21071,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="362" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A362">
         <v>202304</v>
       </c>
@@ -21118,7 +21121,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="363" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A363">
         <v>202304</v>
       </c>
@@ -21168,7 +21171,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="364" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A364">
         <v>202304</v>
       </c>
@@ -21218,7 +21221,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="365" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A365">
         <v>202304</v>
       </c>
@@ -21265,7 +21268,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="366" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A366">
         <v>202304</v>
       </c>
@@ -21318,7 +21321,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="367" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A367">
         <v>202304</v>
       </c>
@@ -21371,7 +21374,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="368" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A368">
         <v>202304</v>
       </c>
@@ -21424,7 +21427,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="369" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A369">
         <v>202304</v>
       </c>
@@ -21483,7 +21486,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="370" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A370">
         <v>202304</v>
       </c>
@@ -21536,7 +21539,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="371" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A371">
         <v>202304</v>
       </c>
@@ -21589,7 +21592,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="372" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A372">
         <v>202304</v>
       </c>
@@ -21642,7 +21645,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="373" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A373">
         <v>202304</v>
       </c>
@@ -21695,7 +21698,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="374" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A374">
         <v>202304</v>
       </c>
@@ -21748,7 +21751,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="375" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A375">
         <v>202304</v>
       </c>
@@ -21801,7 +21804,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="376" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A376">
         <v>202304</v>
       </c>
@@ -21854,7 +21857,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="377" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A377">
         <v>202304</v>
       </c>
@@ -21907,7 +21910,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="378" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A378">
         <v>202304</v>
       </c>
@@ -21966,7 +21969,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="379" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A379">
         <v>202304</v>
       </c>
@@ -22019,7 +22022,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="380" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A380">
         <v>202304</v>
       </c>
@@ -22072,7 +22075,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="381" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A381">
         <v>202304</v>
       </c>
@@ -22128,7 +22131,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="382" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A382">
         <v>202304</v>
       </c>
@@ -22187,7 +22190,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="383" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A383">
         <v>202304</v>
       </c>
@@ -22246,7 +22249,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="384" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A384">
         <v>202304</v>
       </c>
@@ -22299,7 +22302,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="385" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A385">
         <v>202304</v>
       </c>
@@ -22352,7 +22355,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="386" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A386">
         <v>202304</v>
       </c>
@@ -22405,7 +22408,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="387" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A387">
         <v>202304</v>
       </c>
@@ -22461,7 +22464,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="388" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A388">
         <v>202304</v>
       </c>
@@ -22520,7 +22523,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="389" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A389">
         <v>202304</v>
       </c>
@@ -22573,7 +22576,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="390" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A390">
         <v>202304</v>
       </c>
@@ -22626,7 +22629,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="391" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A391">
         <v>202304</v>
       </c>
@@ -22679,7 +22682,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="392" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A392">
         <v>202304</v>
       </c>
@@ -22735,7 +22738,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="393" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A393">
         <v>202304</v>
       </c>
@@ -22788,7 +22791,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="394" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A394">
         <v>202304</v>
       </c>
@@ -22841,7 +22844,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="395" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A395">
         <v>202304</v>
       </c>
@@ -22894,7 +22897,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="396" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A396">
         <v>202304</v>
       </c>
@@ -22947,7 +22950,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="397" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A397">
         <v>202304</v>
       </c>
@@ -23000,7 +23003,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="398" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A398">
         <v>202304</v>
       </c>
@@ -23053,7 +23056,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="399" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A399">
         <v>202304</v>
       </c>
@@ -23109,7 +23112,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="400" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A400">
         <v>202304</v>
       </c>

</xml_diff>